<commit_message>
average cost results: New results after bug corrections.
</commit_message>
<xml_diff>
--- a/results/Average cost.xlsx
+++ b/results/Average cost.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="25120" windowHeight="15840" tabRatio="500"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="25120" windowHeight="15900" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,10 +43,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -69,13 +85,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -151,22 +179,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>72.0</c:v>
+                  <c:v>144.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>81.0</c:v>
+                  <c:v>162.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>85.0</c:v>
+                  <c:v>170.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>113.0</c:v>
+                  <c:v>226.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>137.0</c:v>
+                  <c:v>274.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>172.0</c:v>
+                  <c:v>344.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -221,22 +249,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>70.0</c:v>
+                  <c:v>135.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>78.0</c:v>
+                  <c:v>155.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>82.0</c:v>
+                  <c:v>162.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>108.0</c:v>
+                  <c:v>218.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>130.0</c:v>
+                  <c:v>265.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>163.0</c:v>
+                  <c:v>332.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -291,22 +319,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>81.0</c:v>
+                  <c:v>166.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>93.0</c:v>
+                  <c:v>187.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>99.0</c:v>
+                  <c:v>196.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>129.0</c:v>
+                  <c:v>260.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>155.0</c:v>
+                  <c:v>317.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>193.0</c:v>
+                  <c:v>398.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -361,22 +389,22 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>78.0</c:v>
+                  <c:v>161.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>89.0</c:v>
+                  <c:v>181.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>95.0</c:v>
+                  <c:v>191.0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>121.0</c:v>
+                  <c:v>253.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>147.0</c:v>
+                  <c:v>307.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>186.0</c:v>
+                  <c:v>385.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -393,11 +421,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2096035048"/>
-        <c:axId val="-2124748536"/>
+        <c:axId val="2124955832"/>
+        <c:axId val="2124962904"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2096035048"/>
+        <c:axId val="2124955832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -430,7 +458,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2124748536"/>
+        <c:crossAx val="2124962904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -438,11 +466,11 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2124748536"/>
+        <c:axId val="2124962904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="200.0"/>
-          <c:min val="60.0"/>
+          <c:max val="400.0"/>
+          <c:min val="130.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -470,9 +498,10 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2096035048"/>
+        <c:crossAx val="2124955832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
+        <c:majorUnit val="30.0"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -496,16 +525,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>50800</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -852,7 +881,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -888,16 +917,16 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>72</v>
+        <v>144</v>
       </c>
       <c r="D2">
-        <v>70</v>
+        <v>135</v>
       </c>
       <c r="E2">
-        <v>81</v>
+        <v>166</v>
       </c>
       <c r="F2">
-        <v>78</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -905,16 +934,16 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="D3">
-        <v>78</v>
+        <v>155</v>
       </c>
       <c r="E3">
-        <v>93</v>
+        <v>187</v>
       </c>
       <c r="F3">
-        <v>89</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -922,16 +951,16 @@
         <v>15</v>
       </c>
       <c r="C4">
-        <v>85</v>
+        <v>170</v>
       </c>
       <c r="D4">
-        <v>82</v>
+        <v>162</v>
       </c>
       <c r="E4">
-        <v>99</v>
+        <v>196</v>
       </c>
       <c r="F4">
-        <v>95</v>
+        <v>191</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -939,16 +968,16 @@
         <v>20</v>
       </c>
       <c r="C5">
-        <v>113</v>
+        <v>226</v>
       </c>
       <c r="D5">
-        <v>108</v>
+        <v>218</v>
       </c>
       <c r="E5">
-        <v>129</v>
+        <v>260</v>
       </c>
       <c r="F5">
-        <v>121</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -956,16 +985,16 @@
         <v>25</v>
       </c>
       <c r="C6">
-        <v>137</v>
+        <v>274</v>
       </c>
       <c r="D6">
-        <v>130</v>
+        <v>265</v>
       </c>
       <c r="E6">
-        <v>155</v>
+        <v>317</v>
       </c>
       <c r="F6">
-        <v>147</v>
+        <v>307</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -973,20 +1002,21 @@
         <v>30</v>
       </c>
       <c r="C7">
-        <v>172</v>
+        <v>344</v>
       </c>
       <c r="D7">
-        <v>163</v>
+        <v>332</v>
       </c>
       <c r="E7">
-        <v>193</v>
+        <v>398</v>
       </c>
       <c r="F7">
-        <v>186</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>